<commit_message>
first version based on a table plus some research
</commit_message>
<xml_diff>
--- a/data/data-sheet-example.xlsx
+++ b/data/data-sheet-example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1960" yWindow="3420" windowWidth="25600" windowHeight="12980" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="0" windowWidth="21580" windowHeight="16580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,104 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+  <si>
+    <t>6.0</t>
+  </si>
+  <si>
+    <t>11.4</t>
+  </si>
+  <si>
+    <t>10.4</t>
+  </si>
+  <si>
+    <t>9.5</t>
+  </si>
+  <si>
+    <t>8.8</t>
+  </si>
+  <si>
+    <t>8.1</t>
+  </si>
+  <si>
+    <t>7.6</t>
+  </si>
+  <si>
+    <t>7.1</t>
+  </si>
+  <si>
+    <t>6.7</t>
+  </si>
+  <si>
+    <t>6.3</t>
+  </si>
+  <si>
+    <t>5.7</t>
+  </si>
+  <si>
+    <t>5.4</t>
+  </si>
+  <si>
+    <t>5.2</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>4.7</t>
+  </si>
+  <si>
+    <t>4.6</t>
+  </si>
+  <si>
+    <t>4.4</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>3.9</t>
+  </si>
+  <si>
+    <t>3.8</t>
+  </si>
+  <si>
+    <t>3.7</t>
+  </si>
+  <si>
+    <t>3.6</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>3.4</t>
+  </si>
+  <si>
+    <t>3.3</t>
+  </si>
+  <si>
+    <t>3.2</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>2.9</t>
+  </si>
+  <si>
+    <t>2.8</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -65,17 +163,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -408,7 +510,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:O32"/>
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -467,7 +569,7 @@
         <v>65</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:O2" si="0">$A2+D$1</f>
+        <f t="shared" ref="D2:N2" si="0">$A2+D$1</f>
         <v>70</v>
       </c>
       <c r="E2">
@@ -486,9 +588,8 @@
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="I2">
-        <f t="shared" si="0"/>
-        <v>95</v>
+      <c r="I2" t="s">
+        <v>1</v>
       </c>
       <c r="J2">
         <f t="shared" si="0"/>
@@ -516,7 +617,7 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:O32" si="1">$A3+B$1</f>
+        <f t="shared" ref="B3:N32" si="1">$A3+B$1</f>
         <v>61</v>
       </c>
       <c r="C3">
@@ -543,9 +644,8 @@
         <f t="shared" si="1"/>
         <v>91</v>
       </c>
-      <c r="I3">
-        <f t="shared" si="1"/>
-        <v>96</v>
+      <c r="I3" t="s">
+        <v>2</v>
       </c>
       <c r="J3">
         <f t="shared" si="1"/>
@@ -600,9 +700,8 @@
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
-      <c r="I4">
-        <f t="shared" si="1"/>
-        <v>97</v>
+      <c r="I4" t="s">
+        <v>3</v>
       </c>
       <c r="J4">
         <f t="shared" si="1"/>
@@ -657,9 +756,8 @@
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
-      <c r="I5">
-        <f t="shared" si="1"/>
-        <v>98</v>
+      <c r="I5" t="s">
+        <v>4</v>
       </c>
       <c r="J5">
         <f t="shared" si="1"/>
@@ -714,9 +812,8 @@
         <f t="shared" si="1"/>
         <v>94</v>
       </c>
-      <c r="I6">
-        <f t="shared" si="1"/>
-        <v>99</v>
+      <c r="I6" t="s">
+        <v>5</v>
       </c>
       <c r="J6">
         <f t="shared" si="1"/>
@@ -771,9 +868,8 @@
         <f t="shared" si="1"/>
         <v>95</v>
       </c>
-      <c r="I7">
-        <f t="shared" si="1"/>
-        <v>100</v>
+      <c r="I7" t="s">
+        <v>6</v>
       </c>
       <c r="J7">
         <f t="shared" si="1"/>
@@ -828,9 +924,8 @@
         <f t="shared" si="1"/>
         <v>96</v>
       </c>
-      <c r="I8">
-        <f t="shared" si="1"/>
-        <v>101</v>
+      <c r="I8" t="s">
+        <v>7</v>
       </c>
       <c r="J8">
         <f t="shared" si="1"/>
@@ -885,9 +980,8 @@
         <f t="shared" si="1"/>
         <v>97</v>
       </c>
-      <c r="I9">
-        <f t="shared" si="1"/>
-        <v>102</v>
+      <c r="I9" t="s">
+        <v>8</v>
       </c>
       <c r="J9">
         <f t="shared" si="1"/>
@@ -942,9 +1036,8 @@
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
-      <c r="I10">
-        <f t="shared" si="1"/>
-        <v>103</v>
+      <c r="I10" t="s">
+        <v>9</v>
       </c>
       <c r="J10">
         <f t="shared" si="1"/>
@@ -999,9 +1092,8 @@
         <f t="shared" si="1"/>
         <v>99</v>
       </c>
-      <c r="I11">
-        <f t="shared" si="1"/>
-        <v>104</v>
+      <c r="I11" t="s">
+        <v>0</v>
       </c>
       <c r="J11">
         <f t="shared" si="1"/>
@@ -1056,9 +1148,8 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="I12">
-        <f t="shared" si="1"/>
-        <v>105</v>
+      <c r="I12" t="s">
+        <v>10</v>
       </c>
       <c r="J12">
         <f t="shared" si="1"/>
@@ -1113,9 +1204,8 @@
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
-      <c r="I13">
-        <f t="shared" si="1"/>
-        <v>106</v>
+      <c r="I13" t="s">
+        <v>11</v>
       </c>
       <c r="J13">
         <f t="shared" si="1"/>
@@ -1170,9 +1260,8 @@
         <f t="shared" si="1"/>
         <v>102</v>
       </c>
-      <c r="I14">
-        <f t="shared" si="1"/>
-        <v>107</v>
+      <c r="I14" t="s">
+        <v>12</v>
       </c>
       <c r="J14">
         <f t="shared" si="1"/>
@@ -1227,9 +1316,8 @@
         <f t="shared" si="1"/>
         <v>103</v>
       </c>
-      <c r="I15">
-        <f t="shared" si="1"/>
-        <v>108</v>
+      <c r="I15" t="s">
+        <v>13</v>
       </c>
       <c r="J15">
         <f t="shared" si="1"/>
@@ -1284,9 +1372,8 @@
         <f t="shared" si="1"/>
         <v>104</v>
       </c>
-      <c r="I16">
-        <f t="shared" si="1"/>
-        <v>109</v>
+      <c r="I16" t="s">
+        <v>14</v>
       </c>
       <c r="J16">
         <f t="shared" si="1"/>
@@ -1341,9 +1428,8 @@
         <f t="shared" si="1"/>
         <v>105</v>
       </c>
-      <c r="I17">
-        <f t="shared" si="1"/>
-        <v>110</v>
+      <c r="I17" t="s">
+        <v>15</v>
       </c>
       <c r="J17">
         <f t="shared" si="1"/>
@@ -1398,9 +1484,8 @@
         <f t="shared" si="1"/>
         <v>106</v>
       </c>
-      <c r="I18">
-        <f t="shared" si="1"/>
-        <v>111</v>
+      <c r="I18" t="s">
+        <v>16</v>
       </c>
       <c r="J18">
         <f t="shared" si="1"/>
@@ -1448,16 +1533,15 @@
         <v>97</v>
       </c>
       <c r="G19">
-        <f t="shared" ref="D19:O32" si="2">$A19+G$1</f>
+        <f t="shared" ref="D19:N32" si="2">$A19+G$1</f>
         <v>102</v>
       </c>
       <c r="H19">
         <f t="shared" si="2"/>
         <v>107</v>
       </c>
-      <c r="I19">
-        <f t="shared" si="2"/>
-        <v>112</v>
+      <c r="I19" t="s">
+        <v>17</v>
       </c>
       <c r="J19">
         <f t="shared" si="2"/>
@@ -1512,9 +1596,8 @@
         <f t="shared" si="2"/>
         <v>108</v>
       </c>
-      <c r="I20">
-        <f t="shared" si="2"/>
-        <v>113</v>
+      <c r="I20" t="s">
+        <v>18</v>
       </c>
       <c r="J20">
         <f t="shared" si="2"/>
@@ -1569,9 +1652,8 @@
         <f t="shared" si="2"/>
         <v>109</v>
       </c>
-      <c r="I21">
-        <f t="shared" si="2"/>
-        <v>114</v>
+      <c r="I21" t="s">
+        <v>19</v>
       </c>
       <c r="J21">
         <f t="shared" si="2"/>
@@ -1626,9 +1708,8 @@
         <f t="shared" si="2"/>
         <v>110</v>
       </c>
-      <c r="I22">
-        <f t="shared" si="2"/>
-        <v>115</v>
+      <c r="I22" t="s">
+        <v>20</v>
       </c>
       <c r="J22">
         <f t="shared" si="2"/>
@@ -1683,9 +1764,8 @@
         <f t="shared" si="2"/>
         <v>111</v>
       </c>
-      <c r="I23">
-        <f t="shared" si="2"/>
-        <v>116</v>
+      <c r="I23" t="s">
+        <v>21</v>
       </c>
       <c r="J23">
         <f t="shared" si="2"/>
@@ -1740,9 +1820,8 @@
         <f t="shared" si="2"/>
         <v>112</v>
       </c>
-      <c r="I24">
-        <f t="shared" si="2"/>
-        <v>117</v>
+      <c r="I24" t="s">
+        <v>22</v>
       </c>
       <c r="J24">
         <f t="shared" si="2"/>
@@ -1797,9 +1876,8 @@
         <f t="shared" si="2"/>
         <v>113</v>
       </c>
-      <c r="I25">
-        <f t="shared" si="2"/>
-        <v>118</v>
+      <c r="I25" t="s">
+        <v>23</v>
       </c>
       <c r="J25">
         <f t="shared" si="2"/>
@@ -1854,9 +1932,8 @@
         <f t="shared" si="2"/>
         <v>114</v>
       </c>
-      <c r="I26">
-        <f t="shared" si="2"/>
-        <v>119</v>
+      <c r="I26" t="s">
+        <v>24</v>
       </c>
       <c r="J26">
         <f t="shared" si="2"/>
@@ -1911,9 +1988,8 @@
         <f t="shared" si="2"/>
         <v>115</v>
       </c>
-      <c r="I27">
-        <f t="shared" si="2"/>
-        <v>120</v>
+      <c r="I27" t="s">
+        <v>25</v>
       </c>
       <c r="J27">
         <f t="shared" si="2"/>
@@ -1968,9 +2044,8 @@
         <f t="shared" si="2"/>
         <v>116</v>
       </c>
-      <c r="I28">
-        <f t="shared" si="2"/>
-        <v>121</v>
+      <c r="I28" t="s">
+        <v>26</v>
       </c>
       <c r="J28">
         <f t="shared" si="2"/>
@@ -2025,9 +2100,8 @@
         <f t="shared" si="2"/>
         <v>117</v>
       </c>
-      <c r="I29">
-        <f t="shared" si="2"/>
-        <v>122</v>
+      <c r="I29" t="s">
+        <v>27</v>
       </c>
       <c r="J29">
         <f t="shared" si="2"/>
@@ -2082,9 +2156,8 @@
         <f t="shared" si="2"/>
         <v>118</v>
       </c>
-      <c r="I30">
-        <f t="shared" si="2"/>
-        <v>123</v>
+      <c r="I30" t="s">
+        <v>28</v>
       </c>
       <c r="J30">
         <f t="shared" si="2"/>
@@ -2139,9 +2212,8 @@
         <f t="shared" si="2"/>
         <v>119</v>
       </c>
-      <c r="I31">
-        <f t="shared" si="2"/>
-        <v>124</v>
+      <c r="I31" t="s">
+        <v>29</v>
       </c>
       <c r="J31">
         <f t="shared" si="2"/>
@@ -2196,9 +2268,8 @@
         <f t="shared" si="2"/>
         <v>120</v>
       </c>
-      <c r="I32">
-        <f t="shared" si="2"/>
-        <v>125</v>
+      <c r="I32" t="s">
+        <v>30</v>
       </c>
       <c r="J32">
         <f t="shared" si="2"/>

</xml_diff>